<commit_message>
data update and sports bike
</commit_message>
<xml_diff>
--- a/data/mk8 data.xlsx
+++ b/data/mk8 data.xlsx
@@ -214,18 +214,12 @@
     <t>Slick</t>
   </si>
   <si>
-    <t>Rollers</t>
-  </si>
-  <si>
     <t>Slim</t>
   </si>
   <si>
     <t>Metal</t>
   </si>
   <si>
-    <t>Cream Blocks</t>
-  </si>
-  <si>
     <t>Wood</t>
   </si>
   <si>
@@ -326,6 +320,12 @@
   </si>
   <si>
     <t>red = Sport Bike</t>
+  </si>
+  <si>
+    <t>Roller</t>
+  </si>
+  <si>
+    <t>Retro Off-Road</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +443,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -919,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1160,15 +1166,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1178,6 +1175,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1481,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,14 +1498,14 @@
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>6</v>
@@ -1536,6 +1543,7 @@
       <c r="O4" s="81" t="s">
         <v>5</v>
       </c>
+      <c r="P4" s="148"/>
       <c r="Q4" s="10" t="s">
         <v>61</v>
       </c>
@@ -1555,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Y4" s="19" t="s">
         <v>1</v>
@@ -1575,7 +1583,7 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>7</v>
@@ -1613,8 +1621,9 @@
       <c r="O5" s="83">
         <v>4.5</v>
       </c>
+      <c r="P5" s="148"/>
       <c r="Q5" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R5" s="20">
         <v>1.25</v>
@@ -1652,7 +1661,7 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>8</v>
@@ -1690,8 +1699,9 @@
       <c r="O6" s="83">
         <v>4.5</v>
       </c>
+      <c r="P6" s="148"/>
       <c r="Q6" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R6" s="20"/>
       <c r="S6" s="15"/>
@@ -1699,7 +1709,7 @@
       <c r="U6" s="15"/>
       <c r="V6" s="16"/>
       <c r="X6" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Y6" s="21">
         <v>0</v>
@@ -1719,7 +1729,7 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>9</v>
@@ -1757,16 +1767,17 @@
       <c r="O7" s="83">
         <v>4.5</v>
       </c>
+      <c r="P7" s="148"/>
       <c r="Q7" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R7" s="20"/>
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
       <c r="V7" s="16"/>
-      <c r="X7" s="146" t="s">
-        <v>71</v>
+      <c r="X7" s="143" t="s">
+        <v>69</v>
       </c>
       <c r="Y7" s="21">
         <v>0</v>
@@ -1786,7 +1797,7 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>10</v>
@@ -1824,8 +1835,9 @@
       <c r="O8" s="83">
         <v>4.5</v>
       </c>
+      <c r="P8" s="148"/>
       <c r="Q8" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R8" s="20"/>
       <c r="S8" s="15"/>
@@ -1833,7 +1845,7 @@
       <c r="U8" s="15"/>
       <c r="V8" s="16"/>
       <c r="X8" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y8" s="21">
         <v>0</v>
@@ -1852,8 +1864,8 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="147" t="s">
-        <v>102</v>
+      <c r="A9" s="144" t="s">
+        <v>100</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>11</v>
@@ -1891,8 +1903,9 @@
       <c r="O9" s="83">
         <v>4.5</v>
       </c>
+      <c r="P9" s="148"/>
       <c r="Q9" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R9" s="20"/>
       <c r="S9" s="15"/>
@@ -1900,7 +1913,7 @@
       <c r="U9" s="15"/>
       <c r="V9" s="16"/>
       <c r="X9" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Y9" s="20">
         <v>0</v>
@@ -1955,8 +1968,9 @@
       <c r="O10" s="83">
         <v>4.5</v>
       </c>
+      <c r="P10" s="148"/>
       <c r="Q10" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R10" s="20">
         <v>-0.25</v>
@@ -1974,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Y10" s="21">
         <v>0</v>
@@ -2012,7 +2026,7 @@
         <v>0.5</v>
       </c>
       <c r="J11" s="99" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K11" s="100">
         <v>2.25</v>
@@ -2029,8 +2043,9 @@
       <c r="O11" s="101">
         <v>4.5</v>
       </c>
+      <c r="P11" s="148"/>
       <c r="Q11" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R11" s="20"/>
       <c r="S11" s="15"/>
@@ -2038,7 +2053,7 @@
       <c r="U11" s="15"/>
       <c r="V11" s="16"/>
       <c r="X11" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Y11" s="21">
         <v>0</v>
@@ -2057,7 +2072,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="145" t="s">
+      <c r="C12" s="142" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="21">
@@ -2093,8 +2108,9 @@
       <c r="O12" s="104">
         <v>4.25</v>
       </c>
+      <c r="P12" s="148"/>
       <c r="Q12" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R12" s="20"/>
       <c r="S12" s="15"/>
@@ -2102,7 +2118,7 @@
       <c r="U12" s="15"/>
       <c r="V12" s="16"/>
       <c r="X12" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Y12" s="21">
         <v>0</v>
@@ -2121,7 +2137,7 @@
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="145" t="s">
+      <c r="C13" s="142" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="21">
@@ -2157,8 +2173,9 @@
       <c r="O13" s="85">
         <v>4.25</v>
       </c>
+      <c r="P13" s="148"/>
       <c r="Q13" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R13" s="20"/>
       <c r="S13" s="15"/>
@@ -2166,7 +2183,7 @@
       <c r="U13" s="15"/>
       <c r="V13" s="16"/>
       <c r="X13" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Y13" s="21">
         <v>0</v>
@@ -2185,8 +2202,8 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="145" t="s">
-        <v>85</v>
+      <c r="C14" s="142" t="s">
+        <v>83</v>
       </c>
       <c r="D14" s="21">
         <v>-0.75</v>
@@ -2221,8 +2238,9 @@
       <c r="O14" s="85">
         <v>4.25</v>
       </c>
+      <c r="P14" s="148"/>
       <c r="Q14" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R14" s="20"/>
       <c r="S14" s="15"/>
@@ -2230,7 +2248,7 @@
       <c r="U14" s="15"/>
       <c r="V14" s="16"/>
       <c r="X14" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Y14" s="21">
         <v>0</v>
@@ -2249,7 +2267,7 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="145" t="s">
+      <c r="C15" s="142" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="21">
@@ -2285,6 +2303,7 @@
       <c r="O15" s="85">
         <v>4.25</v>
       </c>
+      <c r="P15" s="148"/>
       <c r="Q15" s="25" t="s">
         <v>62</v>
       </c>
@@ -2305,7 +2324,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="145" t="s">
+      <c r="C16" s="142" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="21">
@@ -2341,8 +2360,9 @@
       <c r="O16" s="85">
         <v>4.25</v>
       </c>
+      <c r="P16" s="148"/>
       <c r="Q16" s="23" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="R16" s="21">
         <v>0</v>
@@ -2361,8 +2381,8 @@
       </c>
     </row>
     <row r="17" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="145" t="s">
-        <v>86</v>
+      <c r="C17" s="142" t="s">
+        <v>84</v>
       </c>
       <c r="D17" s="21">
         <v>0.25</v>
@@ -2397,6 +2417,7 @@
       <c r="O17" s="85">
         <v>4.25</v>
       </c>
+      <c r="P17" s="148"/>
       <c r="Q17" s="23" t="s">
         <v>63</v>
       </c>
@@ -2417,8 +2438,8 @@
       </c>
     </row>
     <row r="18" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="145" t="s">
-        <v>87</v>
+      <c r="C18" s="142" t="s">
+        <v>85</v>
       </c>
       <c r="D18" s="22">
         <v>0.5</v>
@@ -2453,8 +2474,9 @@
       <c r="O18" s="107">
         <v>4.25</v>
       </c>
+      <c r="P18" s="148"/>
       <c r="Q18" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R18" s="21">
         <v>0.25</v>
@@ -2473,12 +2495,12 @@
       </c>
     </row>
     <row r="19" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="138"/>
-      <c r="D19" s="139"/>
-      <c r="E19" s="139"/>
-      <c r="F19" s="139"/>
-      <c r="G19" s="139"/>
-      <c r="H19" s="140"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
+      <c r="H19" s="147"/>
       <c r="J19" s="108" t="s">
         <v>41</v>
       </c>
@@ -2497,8 +2519,9 @@
       <c r="O19" s="110">
         <v>4</v>
       </c>
+      <c r="P19" s="148"/>
       <c r="Q19" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R19" s="21">
         <v>0.25</v>
@@ -2553,6 +2576,7 @@
       <c r="O20" s="87">
         <v>4</v>
       </c>
+      <c r="P20" s="148"/>
       <c r="Q20" s="23" t="s">
         <v>64</v>
       </c>
@@ -2573,22 +2597,22 @@
       </c>
     </row>
     <row r="21" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="141" t="s">
+      <c r="C21" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="142">
-        <v>0</v>
-      </c>
-      <c r="E21" s="143">
+      <c r="D21" s="139">
+        <v>0</v>
+      </c>
+      <c r="E21" s="140">
         <v>0.75</v>
       </c>
-      <c r="F21" s="143">
+      <c r="F21" s="140">
         <v>-0.25</v>
       </c>
-      <c r="G21" s="143">
+      <c r="G21" s="140">
         <v>0.75</v>
       </c>
-      <c r="H21" s="144">
+      <c r="H21" s="141">
         <v>-1.25</v>
       </c>
       <c r="J21" s="86" t="s">
@@ -2609,8 +2633,9 @@
       <c r="O21" s="87">
         <v>4</v>
       </c>
+      <c r="P21" s="148"/>
       <c r="Q21" s="24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R21" s="22">
         <v>-0.25</v>
@@ -2629,26 +2654,26 @@
       </c>
     </row>
     <row r="22" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="141" t="s">
+      <c r="C22" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="142">
-        <v>0</v>
-      </c>
-      <c r="E22" s="143">
+      <c r="D22" s="139">
+        <v>0</v>
+      </c>
+      <c r="E22" s="140">
         <v>0.75</v>
       </c>
-      <c r="F22" s="143">
+      <c r="F22" s="140">
         <v>-0.25</v>
       </c>
-      <c r="G22" s="143">
+      <c r="G22" s="140">
         <v>0.75</v>
       </c>
-      <c r="H22" s="144">
+      <c r="H22" s="141">
         <v>1.25</v>
       </c>
       <c r="J22" s="111" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K22" s="112">
         <v>3.25</v>
@@ -2665,8 +2690,9 @@
       <c r="O22" s="113">
         <v>4</v>
       </c>
+      <c r="P22" s="148"/>
       <c r="Q22" s="23" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="R22" s="21">
         <v>-0.5</v>
@@ -2685,22 +2711,22 @@
       </c>
     </row>
     <row r="23" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="141" t="s">
+      <c r="C23" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="142">
-        <v>0</v>
-      </c>
-      <c r="E23" s="143">
+      <c r="D23" s="139">
+        <v>0</v>
+      </c>
+      <c r="E23" s="140">
         <v>0.75</v>
       </c>
-      <c r="F23" s="143">
+      <c r="F23" s="140">
         <v>-0.25</v>
       </c>
-      <c r="G23" s="143">
+      <c r="G23" s="140">
         <v>0.75</v>
       </c>
-      <c r="H23" s="144">
+      <c r="H23" s="141">
         <v>-1.25</v>
       </c>
       <c r="J23" s="114" t="s">
@@ -2721,24 +2747,25 @@
       <c r="O23" s="116">
         <v>3.75</v>
       </c>
+      <c r="P23" s="148"/>
     </row>
     <row r="24" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="141" t="s">
+      <c r="C24" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="142">
-        <v>0</v>
-      </c>
-      <c r="E24" s="143">
+      <c r="D24" s="139">
+        <v>0</v>
+      </c>
+      <c r="E24" s="140">
         <v>0.75</v>
       </c>
-      <c r="F24" s="143">
+      <c r="F24" s="140">
         <v>-0.25</v>
       </c>
-      <c r="G24" s="143">
+      <c r="G24" s="140">
         <v>0.75</v>
       </c>
-      <c r="H24" s="144">
+      <c r="H24" s="141">
         <v>-1.25</v>
       </c>
       <c r="J24" s="88" t="s">
@@ -2759,6 +2786,7 @@
       <c r="O24" s="89">
         <v>3.75</v>
       </c>
+      <c r="P24" s="148"/>
     </row>
     <row r="25" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="14" t="s">
@@ -2838,7 +2866,7 @@
     </row>
     <row r="27" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="4">
         <v>-0.75</v>
@@ -3054,7 +3082,7 @@
     </row>
     <row r="33" spans="10:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J33" s="129" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K33" s="130">
         <v>4.25</v>
@@ -3466,7 +3494,7 @@
         <v>4.25</v>
       </c>
       <c r="I9" s="69" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J9" s="45">
         <v>2.25</v>
@@ -3834,7 +3862,7 @@
       <c r="F20" s="20"/>
       <c r="G20" s="26"/>
       <c r="I20" s="70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J20" s="65">
         <v>3.25</v>
@@ -4232,7 +4260,7 @@
         <v>3.25</v>
       </c>
       <c r="I31" s="71" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J31" s="58">
         <v>4.25</v>

</xml_diff>